<commit_message>
Add new files and solved the mistakes
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>Регистрация нового пользователя</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>№</t>
   </si>
@@ -42,31 +39,6 @@
   </si>
   <si>
     <t>Ожидаемый результат</t>
-  </si>
-  <si>
-    <t>Приложение запущено, доступ к интернету.</t>
-  </si>
-  <si>
-    <t>Пользователь успешно зарегистрирован, отображается сообщение об успешной регистрации.</t>
-  </si>
-  <si>
-    <t>1. Открыть страницу регистрации.
-2. Ввести корректные данные (имя, email, пароль).
-3. Нажать кнопку "Зарегистрироваться".</t>
-  </si>
-  <si>
-    <t>Вход с некорректными данными</t>
-  </si>
-  <si>
-    <t>Приложение запущено.</t>
-  </si>
-  <si>
-    <t>1. Открыть страницу входа.
-2. Ввести некорректные данные (неправильный email или пароль).
-3. Нажать кнопку "Войти".</t>
-  </si>
-  <si>
-    <t>Отображается сообщение об ошибке входа.</t>
   </si>
   <si>
     <t>Пользователь авторизован.</t>
@@ -88,26 +60,131 @@
     <t>В списке новостей есть несколько новостей.</t>
   </si>
   <si>
-    <t>В списке новостей есть новость.</t>
-  </si>
-  <si>
-    <t>1. Открыть страницу создания новости.
-2. Ввести название новости и описание.
-3. Нажать кнопку "Создать новость".</t>
-  </si>
-  <si>
-    <t>1. Выбрать новость для удаления.
-2. Нажать кнопку "Удалить".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Новость успешно создана и отображается в списке новостей.
-</t>
-  </si>
-  <si>
     <t>Отображаются новости, соответствующие ключевому слову.</t>
   </si>
   <si>
-    <t>Новость успешно удалена из списка.</t>
+    <t>Успешная авторизация и выход из профиля</t>
+  </si>
+  <si>
+    <t>Открыт экран авторизации</t>
+  </si>
+  <si>
+    <t>1. Ввести валидный логин.
+2. Ввести валидный пароль.
+3. Нажать кнопку "Войти".
+4. Нажать кнопку "Выход".</t>
+  </si>
+  <si>
+    <t>Пользователь успешно авторизован и вышел из профиля.</t>
+  </si>
+  <si>
+    <t>Неуспешная авторизация с невалидным паролем</t>
+  </si>
+  <si>
+    <t>Открыт экран авторизации.</t>
+  </si>
+  <si>
+    <t>1. Ввести валидный логин.
+2. Ввести невалидный пароль.
+3. Нажать кнопку "Войти".</t>
+  </si>
+  <si>
+    <t>Отображается сообщение об ошибке "Неверные учетные данные".</t>
+  </si>
+  <si>
+    <t>Неуспешная авторизация с пустыми полями</t>
+  </si>
+  <si>
+    <t>1. Оставить поля логина и пароля пустыми.
+2. Нажать кнопку "Войти".</t>
+  </si>
+  <si>
+    <t>Отображается сообщение об ошибке "Заполните пустые поля".</t>
+  </si>
+  <si>
+    <t>Авторизация</t>
+  </si>
+  <si>
+    <t>Группа</t>
+  </si>
+  <si>
+    <t>Страница 
+"О приложении"</t>
+  </si>
+  <si>
+    <t>Проверка элементов страницы "О приложении"</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован</t>
+  </si>
+  <si>
+    <t>1. Открыть главное меню.
+2. Выбрать пункт "О приложении".
+3. Проверить отображение заголовка версии.
+4. Проверить отображение политики конфиденциальности.
+5. Проверить отображение условий использования.
+6. Вернуться на предыдущий экран.</t>
+  </si>
+  <si>
+    <t>1. Открыть главное меню.
+2. Выбрать пункт "Новости".
+3. Нажать кнопку "Создать новость".
+4. Заполнить форму (категория, заголовок, текст).
+5. Сохранить новость.</t>
+  </si>
+  <si>
+    <t>Новость успешно создана и отображается в списке.</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован, есть созданная новость</t>
+  </si>
+  <si>
+    <t>1. Открыть главное меню.
+2. Выбрать пункт "Новости".
+3. Нажать кнопку "Удалить" у выбранной новости.</t>
+  </si>
+  <si>
+    <t>Новость удалена из списка.</t>
+  </si>
+  <si>
+    <t>Редактирование новости</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован, есть созданная новость.</t>
+  </si>
+  <si>
+    <t>1. Открыть главное меню.
+2. Выбрать пункт "Новости".
+3. Нажать кнопку "Редактировать" у выбранной новости.
+4. Изменить данные в форме.
+5. Сохранить изменения.</t>
+  </si>
+  <si>
+    <t>Новость отредактирована, изменения отображаются в списке.</t>
+  </si>
+  <si>
+    <t>Страница 
+"Новости"</t>
+  </si>
+  <si>
+    <t>1. Нажать кнопку "Наша миссия".
+2. Проверить отображение элементов на странице.
+3. Нажать на первую стрелку для раскрытия текста.
+4. Проверить отображение текста.</t>
+  </si>
+  <si>
+    <t>Элементы отображаются корректно, текст раскрывается при нажатии на стрелку.</t>
+  </si>
+  <si>
+    <t>Все элементы отображаются коррректно, возврат на предыдущий экран выполнен.</t>
+  </si>
+  <si>
+    <t>Страница 
+"Наша миссия"</t>
+  </si>
+  <si>
+    <t>Проверка страницы 
+"Наша миссия"</t>
   </si>
 </sst>
 </file>
@@ -131,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -155,26 +232,185 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -189,7 +425,7 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -204,7 +440,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -216,37 +452,136 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,128 +863,216 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.08984375" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="41.36328125" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" customWidth="1"/>
-    <col min="5" max="5" width="28.453125" customWidth="1"/>
-    <col min="6" max="6" width="26" customWidth="1"/>
-    <col min="7" max="7" width="37.26953125" customWidth="1"/>
-    <col min="8" max="8" width="38.1796875" customWidth="1"/>
-    <col min="9" max="9" width="65.1796875" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="25.08984375" customWidth="1"/>
+    <col min="4" max="4" width="41.36328125" customWidth="1"/>
+    <col min="5" max="5" width="45.1796875" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="8" width="37.26953125" customWidth="1"/>
+    <col min="9" max="9" width="38.1796875" customWidth="1"/>
+    <col min="10" max="10" width="65.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="28"/>
+      <c r="C4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="38">
+        <v>4</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="33">
         <v>5</v>
       </c>
+      <c r="B6" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    <row r="7" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="35"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="87" x14ac:dyDescent="0.35">
+      <c r="A8" s="35"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>7</v>
+      <c r="F9" s="43" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+    <row r="10" spans="1:6" ht="60.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>24</v>
+      <c r="E10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B2:B4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>